<commit_message>
202108098 2120 updates from tlw87, checkpoint all happy path endpoints working again.
</commit_message>
<xml_diff>
--- a/docs/Project0 Testing.xlsx
+++ b/docs/Project0 Testing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\Project-0\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3048A2FA-EA00-46C3-B47E-4F36A99D0548}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8510F2E2-9813-47DE-89A3-0C60D85AEF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="105" yWindow="3930" windowWidth="27735" windowHeight="10875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="121">
   <si>
     <t>ClientServiceTest</t>
   </si>
@@ -374,6 +374,62 @@
     <t>http://localhost:3005/client_acct/5/account/Checking/10000.23</t>
   </si>
   <si>
+    <t>http://localhost:3005/client_acct/5/account/84073/50655.23</t>
+  </si>
+  <si>
+    <t>clients: Gets all clients VALID request</t>
+  </si>
+  <si>
+    <t>clients: Gets all clients INVALID request</t>
+  </si>
+  <si>
+    <t>DELETE</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/client/5</t>
+  </si>
+  <si>
+    <t>received message client with id 5 and their accounts were deleted</t>
+  </si>
+  <si>
+    <t>received client with id 5 updated client nickname</t>
+  </si>
+  <si>
+    <t>Delete client with VALID id with account (s)</t>
+  </si>
+  <si>
+    <t>"Account number: [00014] for Client with id: [2] removed from database."</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/client_acct/2/account/00014</t>
+  </si>
+  <si>
+    <r>
+      <t>received client with id 5 updated account [</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>96366</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>] account balance</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t>received client with the new account added generated number: [</t>
     </r>
@@ -386,7 +442,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>84073</t>
+      <t>96366</t>
     </r>
     <r>
       <rPr>
@@ -396,33 +452,14 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>]</t>
+      <t>]
+20210809 endpoint start failing, now working</t>
     </r>
   </si>
   <si>
-    <t>http://localhost:3005/client_acct/5/account/84073/50655.23</t>
-  </si>
-  <si>
-    <t>clients: Gets all clients VALID request</t>
-  </si>
-  <si>
-    <t>clients: Gets all clients INVALID request</t>
-  </si>
-  <si>
-    <t>DELETE</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client/5</t>
-  </si>
-  <si>
-    <t>received message client with id 5 and their accounts were deleted</t>
-  </si>
-  <si>
-    <t>received client with id 5 updated client nickname</t>
-  </si>
-  <si>
     <r>
-      <t>received client with id 5 updated account [</t>
+      <t xml:space="preserve">run 2nd time expected CNF message instead:
+</t>
     </r>
     <r>
       <rPr>
@@ -433,24 +470,49 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>84073</t>
+      <t xml:space="preserve">Internal server error
+</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>] account balance</t>
+      <t xml:space="preserve">Client controller needed to check if client exists prior to sending to account services.
+Now receive:
+</t>
     </r>
-  </si>
-  <si>
-    <t>Delete client with VALID id with account (s)</t>
-  </si>
-  <si>
-    <t>"Account number: [00014] for Client with id: [2] removed from database."</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"message": "Client was not found in the database."</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Also account services was not catching ANF exceptions in the calling chain.</t>
+    </r>
+  </si>
+  <si>
+    <t>client: Delete VALID Account for VALID client id, where account DOES NOT belongs to client.</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/client_acct/2/account/00002</t>
+  </si>
+  <si>
+    <t>"Account number: [00002] does not belong to Client with id: [2]"</t>
   </si>
   <si>
     <r>
@@ -477,38 +539,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>sd</t>
-    </r>
-  </si>
-  <si>
-    <t>http://localhost:3005/client_acct/2/account/00014</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">run 2nd time expected CNF message instead:
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Internal server error
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Client controller needed to check if client exists prior to sending to account services.
-Also account services was not catching ANF exceptions in the calling chain.</t>
+      <t>AccountService code rewritten to return status code to ClientController where ClientController can then process the results without having to catch exceptions.</t>
     </r>
   </si>
 </sst>
@@ -517,9 +548,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="000.00"/>
+    <numFmt numFmtId="164" formatCode="000.00"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,6 +580,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -570,10 +608,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -582,7 +620,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -599,6 +637,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1285,13 +1326,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B301E05-46F7-4687-82C9-0C10B4DB514A}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
+      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1333,7 +1374,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>47</v>
@@ -1353,7 +1394,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>47</v>
@@ -1622,24 +1663,24 @@
         <v>94</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>5</v>
-      </c>
-      <c r="B17" s="6" t="s">
+    <row r="17" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>5</v>
+      </c>
+      <c r="B17" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="E17" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="F17" s="6" t="s">
-        <v>104</v>
+      <c r="F17" s="10" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1659,7 +1700,7 @@
         <v>99</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1676,10 +1717,10 @@
         <v>102</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1687,39 +1728,39 @@
         <v>0</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E20" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
         <v>0</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1727,39 +1768,59 @@
         <v>5</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>87</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
         <v>5</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>87</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>115</v>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>5.01</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>119</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
202108098 2211 updates from tlw87, happy paths working adding more Postman tests.
</commit_message>
<xml_diff>
--- a/docs/Project0 Testing.xlsx
+++ b/docs/Project0 Testing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\Project-0\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8510F2E2-9813-47DE-89A3-0C60D85AEF20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE929A43-62E6-4DC1-8051-22614535E3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="3930" windowWidth="27735" windowHeight="10875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="128">
   <si>
     <t>ClientServiceTest</t>
   </si>
@@ -294,9 +294,6 @@
   </si>
   <si>
     <t>client account with VALID client id and a VALID account number belonging to the client</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client_acct/1/account/01234</t>
   </si>
   <si>
     <t>http://localhost:3005/client_acct/1/account/00002</t>
@@ -542,6 +539,30 @@
       <t>AccountService code rewritten to return status code to ClientController where ClientController can then process the results without having to catch exceptions.</t>
     </r>
   </si>
+  <si>
+    <t>client accounts with VALID client id between a REVERSED range parameters</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/client_acct/1/accounts/400/2000</t>
+  </si>
+  <si>
+    <t>"message": "Accounts were not found in the database for the client."</t>
+  </si>
+  <si>
+    <t>client account with INVALID client id and a VALID account number</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/client_acct/500/account/00002</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/client_acct/1/account/00000</t>
+  </si>
+  <si>
+    <t>client: Add client extra parameter</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/client/Michael/Biehn/Kyle Reese/Was Conor's Father</t>
+  </si>
 </sst>
 </file>
 
@@ -588,15 +609,45 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -604,21 +655,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -632,14 +692,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1326,502 +1428,747 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B301E05-46F7-4687-82C9-0C10B4DB514A}">
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F24" sqref="F24"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35" style="7" customWidth="1"/>
-    <col min="4" max="4" width="65.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.5703125" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="65.85546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35" style="5" customWidth="1"/>
+    <col min="4" max="4" width="65.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="77.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="65.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
-        <v>0</v>
-      </c>
-      <c r="B2" s="6" t="s">
+      <c r="A2" s="10">
+        <v>0</v>
+      </c>
+      <c r="B2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D3" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="E3" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
+        <v>5</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
+        <v>5.01</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>10</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>10.01</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>10.02</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>15</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>15.01</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>15.02</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>20</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>20.010000000000002</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>20.02</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>25</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>25.01</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="10">
+        <v>25.02</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>0</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
         <v>0.01</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C3" s="7" t="s">
+      <c r="B19" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>126</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>5</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="10">
+        <v>0</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="10">
+        <v>5</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>96</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E22" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
+        <v>0</v>
+      </c>
+      <c r="B23" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5">
-        <v>5</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="C23" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
+        <v>0</v>
+      </c>
+      <c r="B24" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
+        <v>5</v>
+      </c>
+      <c r="B25" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="10">
+        <v>5</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E26" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="10">
         <v>5.01</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
-        <v>10</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>10.01</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>10.02</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>15</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>15.01</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>15.02</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>20</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>20.010000000000002</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>25</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E14" s="6" t="s">
+      <c r="B27" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="D27" s="13" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>25.01</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>0</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="11">
-        <v>5</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>0</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" s="6" t="s">
-        <v>99</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>5</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="8" t="s">
-        <v>104</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="5">
-        <v>0</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A21" s="5">
-        <v>0</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>108</v>
-      </c>
-      <c r="F21" s="10" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
-        <v>5</v>
-      </c>
-      <c r="B22" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A23" s="5">
-        <v>5</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="F23" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="5">
-        <v>5.01</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C24" s="7" t="s">
+      <c r="E27" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="D24" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E24" s="8" t="s">
+      <c r="F27" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>119</v>
-      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="10"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="13"/>
+      <c r="E28" s="13"/>
+      <c r="F28" s="13"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="12"/>
+      <c r="D29" s="13"/>
+      <c r="E29" s="13"/>
+      <c r="F29" s="13"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="12"/>
+      <c r="D30" s="13"/>
+      <c r="E30" s="13"/>
+      <c r="F30" s="13"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="12"/>
+      <c r="D31" s="13"/>
+      <c r="E31" s="13"/>
+      <c r="F31" s="13"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="12"/>
+      <c r="D32" s="13"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="13"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="10"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="13"/>
+      <c r="E33" s="13"/>
+      <c r="F33" s="13"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="10"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="12"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="10"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="12"/>
+      <c r="D35" s="13"/>
+      <c r="E35" s="13"/>
+      <c r="F35" s="13"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="10"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="13"/>
+      <c r="E36" s="13"/>
+      <c r="F36" s="13"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="10"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="13"/>
+      <c r="E37" s="13"/>
+      <c r="F37" s="13"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="10"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="13"/>
+      <c r="E38" s="13"/>
+      <c r="F38" s="13"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="10"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="13"/>
+      <c r="E39" s="13"/>
+      <c r="F39" s="13"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="10"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="10"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="13"/>
+      <c r="E41" s="13"/>
+      <c r="F41" s="13"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="10"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="13"/>
+      <c r="E42" s="13"/>
+      <c r="F42" s="13"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="10"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="13"/>
+      <c r="E43" s="13"/>
+      <c r="F43" s="13"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="10"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="12"/>
+      <c r="D44" s="13"/>
+      <c r="E44" s="13"/>
+      <c r="F44" s="13"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="10"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="12"/>
+      <c r="D45" s="13"/>
+      <c r="E45" s="13"/>
+      <c r="F45" s="13"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="10"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="13"/>
+      <c r="E46" s="13"/>
+      <c r="F46" s="13"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="10"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="12"/>
+      <c r="D47" s="13"/>
+      <c r="E47" s="13"/>
+      <c r="F47" s="13"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="10"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="12"/>
+      <c r="D48" s="13"/>
+      <c r="E48" s="13"/>
+      <c r="F48" s="13"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="10"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="12"/>
+      <c r="D49" s="13"/>
+      <c r="E49" s="13"/>
+      <c r="F49" s="13"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="10"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="12"/>
+      <c r="D50" s="13"/>
+      <c r="E50" s="13"/>
+      <c r="F50" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
20210811 0609 final updates from tlw8748253 baseline for demo.
</commit_message>
<xml_diff>
--- a/docs/Project0 Testing.xlsx
+++ b/docs/Project0 Testing.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw87\Desktop\Projects\Project-0\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tlw8748253\Desktop\Projects\Project-0\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE929A43-62E6-4DC1-8051-22614535E3C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15525" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="JUnit" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="164">
   <si>
     <t>ClientServiceTest</t>
   </si>
@@ -193,116 +192,31 @@
     <t>/client/client_id</t>
   </si>
   <si>
-    <t>http://localhost:3005/client/4</t>
-  </si>
-  <si>
     <t>Received client with id=4 along with their account information</t>
   </si>
   <si>
-    <t>http://localhost:3005/clients/4</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/clients/500</t>
-  </si>
-  <si>
-    <t>"message": "Client was not found in the database."</t>
-  </si>
-  <si>
     <t>/clients_accts</t>
   </si>
   <si>
     <t>http://localhost:3005/clients_accts</t>
   </si>
   <si>
-    <t>Received all clients in the database</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/clients_acct</t>
-  </si>
-  <si>
-    <t>client accounts with VALID client id</t>
-  </si>
-  <si>
-    <t>Received client with id=4</t>
-  </si>
-  <si>
-    <t>client accounts with INVALID client id</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client_accts/500</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client_accts/4</t>
-  </si>
-  <si>
-    <t>client accounts with INVALID request VALID client id</t>
-  </si>
-  <si>
-    <t>/client_accts/client_id</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client_acct/4</t>
-  </si>
-  <si>
     <t>client accounts with VALID client id between a range</t>
   </si>
   <si>
-    <t>http://localhost:3005/client_acct/1/accounts/2000/400</t>
-  </si>
-  <si>
     <t>/client_accts/client_id/accounts/less_than/greater_than</t>
   </si>
   <si>
     <t>Received client with id=4 and their accounts within the range</t>
   </si>
   <si>
-    <t>http://localhost:3005/client_acct/1/accounts/20/5</t>
-  </si>
-  <si>
     <t>client accounts with VALID client id no records between the range</t>
   </si>
   <si>
-    <t>clients_accts Gets all clients with thier account information VALID</t>
-  </si>
-  <si>
-    <t>clients_accts Gets all clients with thier account information INVALID</t>
-  </si>
-  <si>
-    <t>client with VALID client id</t>
-  </si>
-  <si>
     <t>client with VALID client id INVALID request</t>
   </si>
   <si>
-    <t>clients Get client with INVALID client id</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Internal server error
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"message": "Accounts were not found in the database for the client."
-Was not catching an execption in a calling method.</t>
-    </r>
-  </si>
-  <si>
-    <t>client account with VALID client id and a VALID account number belonging to the client</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client_acct/1/account/00002</t>
-  </si>
-  <si>
     <t>/client_acct/client_id/account/account_number</t>
-  </si>
-  <si>
-    <t>client account with VALID client id and account not found</t>
   </si>
   <si>
     <r>
@@ -332,15 +246,6 @@
     <t>POST</t>
   </si>
   <si>
-    <t>client: Add client</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client/Michael/Biehn/Kyle Reese</t>
-  </si>
-  <si>
-    <t>/client/client_first_name/client_last_name/client_nickname</t>
-  </si>
-  <si>
     <t>client created with no accounts</t>
   </si>
   <si>
@@ -368,16 +273,7 @@
     <t>/client_acct/client_id/account/account_number/account_balance</t>
   </si>
   <si>
-    <t>http://localhost:3005/client_acct/5/account/Checking/10000.23</t>
-  </si>
-  <si>
     <t>http://localhost:3005/client_acct/5/account/84073/50655.23</t>
-  </si>
-  <si>
-    <t>clients: Gets all clients VALID request</t>
-  </si>
-  <si>
-    <t>clients: Gets all clients INVALID request</t>
   </si>
   <si>
     <t>DELETE</t>
@@ -543,35 +439,430 @@
     <t>client accounts with VALID client id between a REVERSED range parameters</t>
   </si>
   <si>
-    <t>http://localhost:3005/client_acct/1/accounts/400/2000</t>
-  </si>
-  <si>
-    <t>"message": "Accounts were not found in the database for the client."</t>
-  </si>
-  <si>
     <t>client account with INVALID client id and a VALID account number</t>
   </si>
   <si>
-    <t>http://localhost:3005/client_acct/500/account/00002</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client_acct/1/account/00000</t>
-  </si>
-  <si>
-    <t>client: Add client extra parameter</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client/Michael/Biehn/Kyle Reese/Was Conor's Father</t>
+    <t>Update an INVALID account number for a VALID client</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/client_acct/5/account/00000/50655.23</t>
+  </si>
+  <si>
+    <t>client: Add client by body</t>
+  </si>
+  <si>
+    <t>/Michael/Biehn/Kyle Reese/Was Conor's Father</t>
+  </si>
+  <si>
+    <t>/Michael/Biehn/Kyle Reese</t>
+  </si>
+  <si>
+    <t>/4</t>
+  </si>
+  <si>
+    <t>/500</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/client_acct</t>
+  </si>
+  <si>
+    <t>Parameters / Body</t>
+  </si>
+  <si>
+    <t>/1/accounts/2000/400</t>
+  </si>
+  <si>
+    <t>/1/accounts/20/5</t>
+  </si>
+  <si>
+    <t>/1/accounts/400/2000</t>
+  </si>
+  <si>
+    <t>/1/account/00002</t>
+  </si>
+  <si>
+    <t>/1/account/00000</t>
+  </si>
+  <si>
+    <t>/500/account/00002</t>
+  </si>
+  <si>
+    <t>client add an account by body</t>
+  </si>
+  <si>
+    <t>/client_acct</t>
+  </si>
+  <si>
+    <t>/5/account/Checking/10000.23</t>
+  </si>
+  <si>
+    <t>/clients/accounts</t>
+  </si>
+  <si>
+    <t>http://localhost:3005/clients/accounts</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Received all clients in the database without their account information</t>
+  </si>
+  <si>
+    <t>clients/accounts Gets all clients with their account information</t>
+  </si>
+  <si>
+    <t>/clients/1/accounts?acct_greater_than=&lt;##&gt;&amp;acct_less_than=&lt;##&gt;</t>
+  </si>
+  <si>
+    <t>/1/accounts?acct_greater_than=400&amp;acct_less_than=2000</t>
+  </si>
+  <si>
+    <t>/clients/client_id</t>
+  </si>
+  <si>
+    <t>Get all clients request VALID request</t>
+  </si>
+  <si>
+    <t>Get all clients request INVALID request</t>
+  </si>
+  <si>
+    <t>Get all clients with thier account information BYPASS</t>
+  </si>
+  <si>
+    <t>Get a client by VALID client id without accounts</t>
+  </si>
+  <si>
+    <t>Received client with id=4, without accounts</t>
+  </si>
+  <si>
+    <t>/abc</t>
+  </si>
+  <si>
+    <t>Get a client by INVALID characters client id without accounts</t>
+  </si>
+  <si>
+    <t>Get a client by INVALID client id does not exist without accounts</t>
+  </si>
+  <si>
+    <r>
+      <t>"message"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Client was not found in the database."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"message"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Client Id must be a number."</t>
+    </r>
+  </si>
+  <si>
+    <t>Get a client by VALID client id with accounts</t>
+  </si>
+  <si>
+    <t>Get a client by VALID client id with accounts INVALID request</t>
+  </si>
+  <si>
+    <t>Get a client by INVALID characters client id with accounts</t>
+  </si>
+  <si>
+    <t>Get a client by INVALID client id does not exist with accounts</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Internal server error
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Fixed issue: was not catching an execption in a calling method.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"message": "Accounts were not found in the database for the client."</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>"message"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Accounts were not found in the database for the client."</t>
+    </r>
+  </si>
+  <si>
+    <t>Get client accounts with VALID client id between a INVALID range</t>
+  </si>
+  <si>
+    <t>/1/accounts?acct_greater_than=5&amp;acct_less_than=20</t>
+  </si>
+  <si>
+    <t>Get client accounts with VALID client id between a INVALID range parameter reversed</t>
+  </si>
+  <si>
+    <t>Get client account with VALID client id and a VALID account number that belongs to the client</t>
+  </si>
+  <si>
+    <t>/client/client_id/account/account_number</t>
+  </si>
+  <si>
+    <t>Received client with an account that belongs to the client</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Internal server error</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Unknown code changes fixed this error.  Received:
+"message": "Account not found in the database for the client."</t>
+    </r>
+  </si>
+  <si>
+    <t>Recived client with accounts with the ranger parameters sent in request.</t>
+  </si>
+  <si>
+    <t>Get client account with INVALID client id and a VALID account number</t>
+  </si>
+  <si>
+    <r>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFA31515"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"message"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Client was not found in the database."</t>
+    </r>
+  </si>
+  <si>
+    <t>/1/account/00003</t>
+  </si>
+  <si>
+    <r>
+      <t>"message"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Account number not assigned to this client."</t>
+    </r>
+  </si>
+  <si>
+    <t>Get client account with VALID client id and a VALID account number that does not belong to client</t>
+  </si>
+  <si>
+    <t>Get client account with INVALID client id and a INVALID account number</t>
+  </si>
+  <si>
+    <t>Add new client all parameters VALID</t>
+  </si>
+  <si>
+    <t>/clients/client_first_name/client_last_name/client_nickname</t>
+  </si>
+  <si>
+    <t>Add client INVALID extra parameter</t>
+  </si>
+  <si>
+    <t>Not found
+Service not found as expected</t>
+  </si>
+  <si>
+    <t>/ /Biehn/Kyle Reese</t>
+  </si>
+  <si>
+    <r>
+      <t>"message"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF0451A5"/>
+        <rFont val="Consolas"/>
+        <family val="3"/>
+      </rPr>
+      <t>"Client first and last name must contain values."</t>
+    </r>
+  </si>
+  <si>
+    <t>/Michael/ /Kyle Reese</t>
+  </si>
+  <si>
+    <t>Add client INVALID parameter first name blank</t>
+  </si>
+  <si>
+    <t>Add client INVALID parameter last name blank</t>
+  </si>
+  <si>
+    <t>Add new client VALID first &amp; last name but no optional nickname</t>
+  </si>
+  <si>
+    <t>/clients/client_first_name/client_last_name</t>
+  </si>
+  <si>
+    <t>/Earl/Boen/</t>
+  </si>
+  <si>
+    <t>client created with no nickname and no accounts</t>
+  </si>
+  <si>
+    <t>{
+    "firstName": "Lance",
+    "lastName": "Henriksen",
+    "nickname": "Detective Hal Vukovich"
+}</t>
+  </si>
+  <si>
+    <t>{
+    "accountNumber": "",
+    "accountType": "Checking",
+    "accountBalance": "10000.23",
+    "clientId": "5"
+}</t>
+  </si>
+  <si>
+    <t>account created for the client id.
+Account number is left blank because it generated by the program.
+Result a new account was added for the client.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -608,8 +899,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFA31515"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0451A5"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -646,6 +955,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -674,7 +989,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -742,6 +1057,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1022,7 +1353,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1030,17 +1361,17 @@
       <selection pane="bottomLeft" activeCell="D2" sqref="D2:D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="73.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1060,7 +1391,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1100,7 +1431,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1120,7 +1451,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1140,7 +1471,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1160,7 +1491,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1180,7 +1511,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1531,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1551,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1240,7 +1571,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1260,7 +1591,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1280,7 +1611,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1300,7 +1631,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1320,7 +1651,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1671,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1360,7 +1691,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1380,7 +1711,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1400,7 +1731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1427,28 +1758,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B301E05-46F7-4687-82C9-0C10B4DB514A}">
-  <dimension ref="A1:F50"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.54296875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35" style="5" customWidth="1"/>
-    <col min="4" max="4" width="65.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="77.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="65.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="4"/>
+    <col min="4" max="4" width="65.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="33.90625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="70.1796875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>42</v>
       </c>
@@ -1464,711 +1796,1100 @@
       <c r="E1" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>0</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>104</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="C2" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E2" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="F2" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="10">
         <v>0.01</v>
       </c>
       <c r="B3" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="12" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="C3" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="25" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G3" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>5</v>
       </c>
       <c r="B4" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="12" t="s">
-        <v>78</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>60</v>
+      <c r="C4" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="23" t="s">
+        <v>56</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F4" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="13" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="10">
-        <v>5.01</v>
+        <v>6</v>
       </c>
       <c r="B5" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="12" t="s">
-        <v>79</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>60</v>
+      <c r="C5" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>110</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="10">
         <v>10</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C6" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C6" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="10">
         <v>10.01</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="13" t="s">
+      <c r="C7" s="26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="10">
         <v>10.02</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C8" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="10">
-        <v>15</v>
+        <v>10.029999999999999</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C9" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G9" s="28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="10">
-        <v>15.01</v>
+        <v>15</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C10" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="10">
-        <v>15.02</v>
+        <v>15.01</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C11" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="D11" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="10">
-        <v>20</v>
+        <v>15.02</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C12" s="26" t="s">
+        <v>130</v>
+      </c>
+      <c r="D12" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="G12" s="28" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="10">
-        <v>20.010000000000002</v>
+        <v>15.03</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="D13" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C13" s="26" t="s">
+        <v>131</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="G13" s="28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
-        <v>20.02</v>
+        <v>20</v>
       </c>
       <c r="B14" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="D14" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>121</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="C14" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
-        <v>25</v>
+        <v>20.010000000000002</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D15" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E15" s="13" t="s">
-        <v>85</v>
-      </c>
-      <c r="F15" s="13"/>
-    </row>
-    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
-        <v>25.01</v>
+        <v>20.02</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>45</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="F16" s="22" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+      <c r="E16" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="G16" s="28" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="10">
-        <v>25.02</v>
+        <v>21</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="12" t="s">
-        <v>123</v>
-      </c>
-      <c r="D17" s="13" t="s">
+      <c r="C17" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="G17" s="16" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="10">
+        <v>21.01</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A19" s="10">
+        <v>21.02</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="26" t="s">
+        <v>136</v>
+      </c>
+      <c r="D19" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="10">
+        <v>25</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E20" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F20" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A21" s="10">
+        <v>25.01</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E21" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="10">
+        <v>25.02</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E22" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="G22" s="29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A23" s="10">
+        <v>25.03</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E23" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="G23" s="27" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="10">
+        <v>25.04</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E24" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A25" s="10">
+        <v>0</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E25" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A26" s="10">
+        <v>0.01</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E26" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E27" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E28" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G28" s="27" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A29" s="10">
+        <v>1</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="E29" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="G29" s="13" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="A30" s="10">
+        <v>1</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E30" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A31" s="17">
+        <v>5</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C31" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="6" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A32" s="17">
+        <v>6</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="C32" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="E32" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>162</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="10">
+        <v>0</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E33" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F33" s="12"/>
+      <c r="G33" s="13" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A34" s="10">
+        <v>5</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="F34" s="18"/>
+      <c r="G34" s="13" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A35" s="10">
+        <v>5.01</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="C35" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="23" t="s">
+        <v>74</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="F35" s="22"/>
+      <c r="G35" s="22" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A36" s="10">
+        <v>0</v>
+      </c>
+      <c r="B36" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E36" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F36" s="18"/>
+      <c r="G36" s="14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
+      <c r="A37" s="10">
+        <v>0</v>
+      </c>
+      <c r="B37" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="F37" s="18"/>
+      <c r="G37" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A38" s="10">
+        <v>5</v>
+      </c>
+      <c r="B38" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C38" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F38" s="18"/>
+      <c r="G38" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="10">
+        <v>5</v>
+      </c>
+      <c r="B39" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C39" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F39" s="18"/>
+      <c r="G39" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A40" s="10">
+        <v>5.01</v>
+      </c>
+      <c r="B40" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="C40" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="E17" s="13" t="s">
-        <v>124</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10">
-        <v>0</v>
-      </c>
-      <c r="B18" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C18" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E18" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="B19" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C19" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>92</v>
-      </c>
-      <c r="E19" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="F19" s="13" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" s="6" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="17">
-        <v>5</v>
-      </c>
-      <c r="B20" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="E20" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="10">
-        <v>0</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="E21" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="F21" s="13" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="10">
-        <v>5</v>
-      </c>
-      <c r="B22" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="C22" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="E22" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="F22" s="13" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="10">
-        <v>0</v>
-      </c>
-      <c r="B23" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C23" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E23" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="F23" s="14" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A24" s="10">
-        <v>0</v>
-      </c>
-      <c r="B24" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C24" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="E24" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="F24" s="18" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="10">
-        <v>5</v>
-      </c>
-      <c r="B25" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C25" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A26" s="10">
-        <v>5</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>110</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="10">
-        <v>5.01</v>
-      </c>
-      <c r="B27" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="C27" s="12" t="s">
-        <v>116</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E27" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="F27" s="13" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="13"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="13"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="10"/>
-      <c r="B29" s="13"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="13"/>
-      <c r="E29" s="13"/>
-      <c r="F29" s="13"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="13"/>
-      <c r="C30" s="12"/>
-      <c r="D30" s="13"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="13"/>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="13"/>
-      <c r="E31" s="13"/>
-      <c r="F31" s="13"/>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="13"/>
-      <c r="E32" s="13"/>
-      <c r="F32" s="13"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="10"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="13"/>
-      <c r="E33" s="13"/>
-      <c r="F33" s="13"/>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="10"/>
-      <c r="B34" s="13"/>
-      <c r="C34" s="12"/>
-      <c r="D34" s="13"/>
-      <c r="E34" s="13"/>
-      <c r="F34" s="13"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="10"/>
-      <c r="B35" s="13"/>
-      <c r="C35" s="12"/>
-      <c r="D35" s="13"/>
-      <c r="E35" s="13"/>
-      <c r="F35" s="13"/>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="10"/>
-      <c r="B36" s="13"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="13"/>
-      <c r="E36" s="13"/>
-      <c r="F36" s="13"/>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="10"/>
-      <c r="B37" s="13"/>
-      <c r="C37" s="12"/>
-      <c r="D37" s="13"/>
-      <c r="E37" s="13"/>
-      <c r="F37" s="13"/>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="10"/>
-      <c r="B38" s="13"/>
-      <c r="C38" s="12"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="10"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="12"/>
-      <c r="D39" s="13"/>
-      <c r="E39" s="13"/>
-      <c r="F39" s="13"/>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="10"/>
-      <c r="B40" s="13"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="13"/>
-      <c r="E40" s="13"/>
-      <c r="F40" s="13"/>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D40" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="F40" s="18"/>
+      <c r="G40" s="13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="10"/>
       <c r="B41" s="13"/>
       <c r="C41" s="12"/>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
-      <c r="F41" s="13"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F41" s="12"/>
+      <c r="G41" s="13"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="10"/>
       <c r="B42" s="13"/>
       <c r="C42" s="12"/>
       <c r="D42" s="13"/>
       <c r="E42" s="13"/>
-      <c r="F42" s="13"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F42" s="12"/>
+      <c r="G42" s="13"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="10"/>
       <c r="B43" s="13"/>
       <c r="C43" s="12"/>
       <c r="D43" s="13"/>
       <c r="E43" s="13"/>
-      <c r="F43" s="13"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F43" s="12"/>
+      <c r="G43" s="13"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="10"/>
       <c r="B44" s="13"/>
       <c r="C44" s="12"/>
       <c r="D44" s="13"/>
       <c r="E44" s="13"/>
-      <c r="F44" s="13"/>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F44" s="12"/>
+      <c r="G44" s="13"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="10"/>
       <c r="B45" s="13"/>
       <c r="C45" s="12"/>
       <c r="D45" s="13"/>
       <c r="E45" s="13"/>
-      <c r="F45" s="13"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F45" s="12"/>
+      <c r="G45" s="13"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="10"/>
       <c r="B46" s="13"/>
       <c r="C46" s="12"/>
       <c r="D46" s="13"/>
       <c r="E46" s="13"/>
-      <c r="F46" s="13"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F46" s="12"/>
+      <c r="G46" s="13"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="10"/>
       <c r="B47" s="13"/>
       <c r="C47" s="12"/>
       <c r="D47" s="13"/>
       <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F47" s="12"/>
+      <c r="G47" s="13"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="10"/>
       <c r="B48" s="13"/>
       <c r="C48" s="12"/>
       <c r="D48" s="13"/>
       <c r="E48" s="13"/>
-      <c r="F48" s="13"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F48" s="12"/>
+      <c r="G48" s="13"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="10"/>
       <c r="B49" s="13"/>
       <c r="C49" s="12"/>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F49" s="12"/>
+      <c r="G49" s="13"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="10"/>
       <c r="B50" s="13"/>
       <c r="C50" s="12"/>
       <c r="D50" s="13"/>
       <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="13"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A51" s="10"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="12"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="12"/>
+      <c r="G51" s="13"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="10"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="12"/>
+      <c r="G52" s="13"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="10"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="12"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="12"/>
+      <c r="G53" s="13"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A54" s="10"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="12"/>
+      <c r="G54" s="13"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A55" s="10"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="13"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A56" s="10"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="12"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="13"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A57" s="10"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="12"/>
+      <c r="D57" s="13"/>
+      <c r="E57" s="13"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="13"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A58" s="10"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="12"/>
+      <c r="D58" s="13"/>
+      <c r="E58" s="13"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="13"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A59" s="10"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="13"/>
+      <c r="E59" s="13"/>
+      <c r="F59" s="12"/>
+      <c r="G59" s="13"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A60" s="10"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="13"/>
+      <c r="E60" s="13"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="13"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A61" s="10"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="13"/>
+      <c r="E61" s="13"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="13"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A62" s="10"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="13"/>
+      <c r="E62" s="13"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="13"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A63" s="10"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="13"/>
+      <c r="E63" s="13"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
20210811 1332 tlw8748253 Project-0 final.
</commit_message>
<xml_diff>
--- a/docs/Project0 Testing.xlsx
+++ b/docs/Project0 Testing.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="164">
   <si>
     <t>ClientServiceTest</t>
   </si>
@@ -214,9 +214,6 @@
   </si>
   <si>
     <t>client with VALID client id INVALID request</t>
-  </si>
-  <si>
-    <t>/client_acct/client_id/account/account_number</t>
   </si>
   <si>
     <r>
@@ -252,36 +249,18 @@
     <t>client add an account</t>
   </si>
   <si>
-    <t>/client_acct/client_id/account/account_type/account_balance</t>
-  </si>
-  <si>
     <t>PUT</t>
   </si>
   <si>
     <t>update client information</t>
   </si>
   <si>
-    <t>http://localhost:3005/client/5/Michael/Biehn/John Connor Kyle Reese is your father</t>
-  </si>
-  <si>
-    <t>/client/client_id/client_first_name/client_last_name/client_nickname</t>
-  </si>
-  <si>
     <t>Update an account for a given client</t>
   </si>
   <si>
-    <t>/client_acct/client_id/account/account_number/account_balance</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client_acct/5/account/84073/50655.23</t>
-  </si>
-  <si>
     <t>DELETE</t>
   </si>
   <si>
-    <t>http://localhost:3005/client/5</t>
-  </si>
-  <si>
     <t>received message client with id 5 and their accounts were deleted</t>
   </si>
   <si>
@@ -292,9 +271,6 @@
   </si>
   <si>
     <t>"Account number: [00014] for Client with id: [2] removed from database."</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client_acct/2/account/00014</t>
   </si>
   <si>
     <r>
@@ -399,12 +375,6 @@
     </r>
   </si>
   <si>
-    <t>client: Delete VALID Account for VALID client id, where account DOES NOT belongs to client.</t>
-  </si>
-  <si>
-    <t>http://localhost:3005/client_acct/2/account/00002</t>
-  </si>
-  <si>
     <t>"Account number: [00002] does not belong to Client with id: [2]"</t>
   </si>
   <si>
@@ -445,9 +415,6 @@
     <t>Update an INVALID account number for a VALID client</t>
   </si>
   <si>
-    <t>http://localhost:3005/client_acct/5/account/00000/50655.23</t>
-  </si>
-  <si>
     <t>client: Add client by body</t>
   </si>
   <si>
@@ -490,9 +457,6 @@
     <t>client add an account by body</t>
   </si>
   <si>
-    <t>/client_acct</t>
-  </si>
-  <si>
     <t>/5/account/Checking/10000.23</t>
   </si>
   <si>
@@ -518,9 +482,6 @@
   </si>
   <si>
     <t>/clients/client_id</t>
-  </si>
-  <si>
-    <t>Get all clients request VALID request</t>
   </si>
   <si>
     <t>Get all clients request INVALID request</t>
@@ -854,6 +815,45 @@
 Account number is left blank because it generated by the program.
 Result a new account was added for the client.</t>
   </si>
+  <si>
+    <t>Get all clients request VALID request without accounts</t>
+  </si>
+  <si>
+    <t>/clients/client_id/account/account_number/account_balance</t>
+  </si>
+  <si>
+    <t>/clients/clients/account/account_type/account_balance</t>
+  </si>
+  <si>
+    <t>/clients/client_id/client_first_name/client_last_name/client_nickname</t>
+  </si>
+  <si>
+    <t>/5/Michael/Biehn/John Connor Kyle Reese is your father</t>
+  </si>
+  <si>
+    <t>/5/account/84073/50655.23</t>
+  </si>
+  <si>
+    <t>/5/account/00000/50655.23</t>
+  </si>
+  <si>
+    <t>/5</t>
+  </si>
+  <si>
+    <t>/clients/client_id/account/account_number</t>
+  </si>
+  <si>
+    <t>/2/account/00014</t>
+  </si>
+  <si>
+    <t>/2/account/00002</t>
+  </si>
+  <si>
+    <t>Delete VALID Account for VALID client id, where account belongs to client.</t>
+  </si>
+  <si>
+    <t>Delete VALID Account for VALID client id, where account DOES NOT belongs to client.</t>
+  </si>
 </sst>
 </file>
 
@@ -862,7 +862,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="000.00"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -916,6 +916,13 @@
       <color rgb="FF0451A5"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -989,7 +996,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1073,6 +1080,13 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1358,7 +1372,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:D19"/>
+      <selection pane="bottomLeft" activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1765,7 +1779,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomRight" activeCell="C33" sqref="C33:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1797,13 +1811,13 @@
         <v>48</v>
       </c>
       <c r="F1" s="9" t="s">
-        <v>100</v>
+        <v>89</v>
       </c>
       <c r="G1" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="10">
         <v>0</v>
       </c>
@@ -1811,7 +1825,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="26" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="D2" s="25" t="s">
         <v>47</v>
@@ -1820,10 +1834,10 @@
         <v>49</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
@@ -1834,7 +1848,7 @@
         <v>45</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>47</v>
@@ -1843,13 +1857,13 @@
         <v>52</v>
       </c>
       <c r="F3" s="12" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10">
         <v>5</v>
       </c>
@@ -1857,7 +1871,7 @@
         <v>45</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="D4" s="23" t="s">
         <v>56</v>
@@ -1866,7 +1880,7 @@
         <v>57</v>
       </c>
       <c r="F4" s="12" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>51</v>
@@ -1880,16 +1894,16 @@
         <v>45</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="G5" s="13" t="s">
         <v>51</v>
@@ -1903,19 +1917,19 @@
         <v>45</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="D6" s="25" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E6" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F6" s="12" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>122</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -1929,13 +1943,13 @@
         <v>62</v>
       </c>
       <c r="D7" s="25" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E7" s="24" t="s">
         <v>52</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G7" s="13" t="s">
         <v>53</v>
@@ -1949,19 +1963,19 @@
         <v>45</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="D8" s="25" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E8" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -1972,19 +1986,19 @@
         <v>45</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>125</v>
+        <v>112</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E9" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F9" s="12" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="G9" s="28" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -1995,16 +2009,16 @@
         <v>45</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>128</v>
+        <v>115</v>
       </c>
       <c r="D10" s="25" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
       <c r="E10" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F10" s="12" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G10" s="13" t="s">
         <v>55</v>
@@ -2018,7 +2032,7 @@
         <v>45</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>129</v>
+        <v>116</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>54</v>
@@ -2027,7 +2041,7 @@
         <v>52</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>53</v>
@@ -2041,7 +2055,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D12" s="25" t="s">
         <v>54</v>
@@ -2050,10 +2064,10 @@
         <v>52</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>123</v>
+        <v>110</v>
       </c>
       <c r="G12" s="28" t="s">
-        <v>127</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2064,7 +2078,7 @@
         <v>45</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="D13" s="25" t="s">
         <v>54</v>
@@ -2073,13 +2087,13 @@
         <v>52</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="G13" s="28" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="10">
         <v>20</v>
       </c>
@@ -2093,16 +2107,16 @@
         <v>59</v>
       </c>
       <c r="E14" s="24" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F14" s="18" t="s">
-        <v>101</v>
+        <v>90</v>
       </c>
       <c r="G14" s="13" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="10">
         <v>20.010000000000002</v>
       </c>
@@ -2116,16 +2130,16 @@
         <v>59</v>
       </c>
       <c r="E15" s="24" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="G15" s="15" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="10">
         <v>20.02</v>
       </c>
@@ -2133,19 +2147,19 @@
         <v>45</v>
       </c>
       <c r="C16" s="22" t="s">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>59</v>
       </c>
       <c r="E16" s="24" t="s">
-        <v>99</v>
+        <v>88</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="G16" s="28" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2159,16 +2173,16 @@
         <v>58</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E17" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="G17" s="16" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2179,19 +2193,19 @@
         <v>45</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E18" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F18" s="12" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="G18" s="27" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -2202,19 +2216,19 @@
         <v>45</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>136</v>
+        <v>123</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="E19" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>135</v>
+        <v>122</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -2225,19 +2239,19 @@
         <v>45</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>137</v>
+        <v>124</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E20" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="G20" s="13" t="s">
-        <v>139</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -2248,19 +2262,19 @@
         <v>45</v>
       </c>
       <c r="C21" s="18" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E21" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F21" s="18" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="G21" s="18" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2271,19 +2285,19 @@
         <v>45</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E22" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="G22" s="29" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -2294,19 +2308,19 @@
         <v>45</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>146</v>
+        <v>133</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E23" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F23" s="12" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="G23" s="27" t="s">
-        <v>145</v>
+        <v>132</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2317,19 +2331,19 @@
         <v>45</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>147</v>
+        <v>134</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>138</v>
+        <v>125</v>
       </c>
       <c r="E24" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F24" s="12" t="s">
-        <v>144</v>
+        <v>131</v>
       </c>
       <c r="G24" s="29" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
@@ -2337,45 +2351,45 @@
         <v>0</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>148</v>
+        <v>135</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="E25" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F25" s="12" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="G25" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A26" s="10">
+      <c r="A26" s="32">
         <v>0.01</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>149</v>
-      </c>
-      <c r="E26" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>136</v>
+      </c>
+      <c r="E26" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>151</v>
+      <c r="F26" s="22" t="s">
+        <v>84</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2383,22 +2397,22 @@
         <v>0.02</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>155</v>
+        <v>142</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="E27" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F27" s="12" t="s">
-        <v>152</v>
+        <v>139</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2406,22 +2420,22 @@
         <v>0.03</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>156</v>
+        <v>143</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>149</v>
+        <v>136</v>
       </c>
       <c r="E28" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F28" s="12" t="s">
-        <v>154</v>
+        <v>141</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>153</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2429,33 +2443,33 @@
         <v>1</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="E29" s="24" t="s">
         <v>49</v>
       </c>
       <c r="F29" s="12" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="G29" s="13" t="s">
-        <v>160</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A30" s="10">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>47</v>
@@ -2464,10 +2478,10 @@
         <v>49</v>
       </c>
       <c r="F30" s="12" t="s">
-        <v>161</v>
+        <v>148</v>
       </c>
       <c r="G30" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="31" spans="1:7" s="6" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -2475,66 +2489,68 @@
         <v>5</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C31" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="E31" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="6" customFormat="1" ht="87" x14ac:dyDescent="0.35">
+      <c r="A32" s="32">
+        <v>6</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="D32" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="E32" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" s="22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A33" s="32">
+        <v>0</v>
+      </c>
+      <c r="B33" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="D31" s="14" t="s">
+      <c r="C33" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="E31" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>109</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="6" customFormat="1" ht="87" x14ac:dyDescent="0.35">
-      <c r="A32" s="17">
-        <v>6</v>
-      </c>
-      <c r="B32" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="C32" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="E32" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>162</v>
-      </c>
-      <c r="G32" s="18" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" s="10">
-        <v>0</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C33" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="D33" s="13" t="s">
+      <c r="D33" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="F33" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="G33" s="23" t="s">
         <v>72</v>
-      </c>
-      <c r="E33" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="13" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -2542,20 +2558,22 @@
         <v>5</v>
       </c>
       <c r="B34" s="20" t="s">
+        <v>67</v>
+      </c>
+      <c r="C34" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="12" t="s">
-        <v>73</v>
-      </c>
       <c r="D34" s="13" t="s">
-        <v>74</v>
-      </c>
-      <c r="E34" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E34" t="s">
+        <v>49</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="G34" s="13" t="s">
         <v>75</v>
-      </c>
-      <c r="F34" s="18"/>
-      <c r="G34" s="13" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2563,20 +2581,22 @@
         <v>5.01</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D35" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="E35" s="23" t="s">
-        <v>93</v>
-      </c>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22" t="s">
-        <v>64</v>
+        <v>67</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>152</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>157</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2584,20 +2604,22 @@
         <v>0</v>
       </c>
       <c r="B36" s="21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D36" s="13" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="E36" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="F36" s="18"/>
+        <v>49</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>158</v>
+      </c>
       <c r="G36" s="14" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="101.5" x14ac:dyDescent="0.35">
@@ -2605,20 +2627,22 @@
         <v>0</v>
       </c>
       <c r="B37" s="21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D37" s="13" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
       <c r="E37" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>158</v>
+      </c>
+      <c r="G37" s="18" t="s">
         <v>77</v>
-      </c>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="29" x14ac:dyDescent="0.35">
@@ -2626,41 +2650,45 @@
         <v>5</v>
       </c>
       <c r="B38" s="21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D38" s="13" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F38" s="18"/>
+        <v>49</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>160</v>
+      </c>
       <c r="G38" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A39" s="10">
         <v>5</v>
       </c>
       <c r="B39" s="21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>80</v>
+        <v>162</v>
       </c>
       <c r="D39" s="13" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F39" s="18"/>
+        <v>49</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>160</v>
+      </c>
       <c r="G39" s="18" t="s">
-        <v>89</v>
+        <v>79</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
@@ -2668,20 +2696,22 @@
         <v>5.01</v>
       </c>
       <c r="B40" s="21" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>86</v>
+        <v>163</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>63</v>
+        <v>159</v>
       </c>
       <c r="E40" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="F40" s="18"/>
+        <v>49</v>
+      </c>
+      <c r="F40" s="18" t="s">
+        <v>161</v>
+      </c>
       <c r="G40" s="13" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>